<commit_message>
Fix Kd e Kc
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -478,19 +478,19 @@
         <v>0.2175678815553797</v>
       </c>
       <c r="C2" t="n">
-        <v>0.984807753012208</v>
+        <v>0.6427876096865394</v>
       </c>
       <c r="D2" t="n">
-        <v>0.2142625365621797</v>
+        <v>0.1398499385295467</v>
       </c>
       <c r="E2" t="n">
         <v>23031.90515141296</v>
       </c>
       <c r="F2" t="n">
-        <v>4934.874419601276</v>
+        <v>3221.010519643452</v>
       </c>
       <c r="G2" t="n">
-        <v>0.04285250731243595</v>
+        <v>0.02796998770590933</v>
       </c>
     </row>
     <row r="3">
@@ -498,22 +498,22 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1773629620793188</v>
+        <v>0.1773629620793186</v>
       </c>
       <c r="C3" t="n">
-        <v>0.984807753012208</v>
+        <v>0.3420201433256688</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1746684201529234</v>
+        <v>0.06066170571103372</v>
       </c>
       <c r="E3" t="n">
         <v>23031.90515141296</v>
       </c>
       <c r="F3" t="n">
-        <v>4022.94648590928</v>
+        <v>1397.154652259455</v>
       </c>
       <c r="G3" t="n">
-        <v>0.02495263145041762</v>
+        <v>0.008665957958719103</v>
       </c>
     </row>
     <row r="4">
@@ -524,19 +524,19 @@
         <v>0.1773629620793188</v>
       </c>
       <c r="C4" t="n">
-        <v>0.984807753012208</v>
+        <v>0.3420201433256687</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1746684201529234</v>
+        <v>0.06066170571103378</v>
       </c>
       <c r="E4" t="n">
         <v>23031.90515141296</v>
       </c>
       <c r="F4" t="n">
-        <v>4022.946485909281</v>
+        <v>1397.154652259456</v>
       </c>
       <c r="G4" t="n">
-        <v>0.01587894728662941</v>
+        <v>0.005514700519184889</v>
       </c>
     </row>
     <row r="5">
@@ -547,19 +547,19 @@
         <v>0.2175678815553798</v>
       </c>
       <c r="C5" t="n">
-        <v>0.984807753012208</v>
+        <v>0.6427876096865394</v>
       </c>
       <c r="D5" t="n">
-        <v>0.2142625365621798</v>
+        <v>0.1398499385295467</v>
       </c>
       <c r="E5" t="n">
         <v>23031.90515141296</v>
       </c>
       <c r="F5" t="n">
-        <v>4934.874419601277</v>
+        <v>3221.010519643452</v>
       </c>
       <c r="G5" t="n">
-        <v>0.01648173358170614</v>
+        <v>0.0107576875791959</v>
       </c>
     </row>
     <row r="6">
@@ -567,22 +567,22 @@
         <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9597950805239389</v>
+        <v>0.9597950805239367</v>
       </c>
       <c r="C6" t="n">
         <v>0.984807753012208</v>
       </c>
       <c r="D6" t="n">
-        <v>0.9452136366029515</v>
+        <v>0.9452136366029493</v>
       </c>
       <c r="E6" t="n">
         <v>23031.90515141296</v>
       </c>
       <c r="F6" t="n">
-        <v>21770.0708260613</v>
+        <v>21770.07082606125</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0556008021531148</v>
+        <v>0.05560080215311466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>